<commit_message>
Removed Unwanted Classes and Codes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Multi User Credentials" sheetId="1" r:id="rId1"/>
+    <sheet name="Single User Credentials" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>testcaseid</t>
   </si>
@@ -45,6 +46,12 @@
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>testcase</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
@@ -365,21 +372,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="10" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.5546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="14" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -389,8 +397,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -400,8 +411,11 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -411,8 +425,11 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>5</v>
       </c>
@@ -421,6 +438,58 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>